<commit_message>
Automation the third test in Class name OpenAccountTest.Java
</commit_message>
<xml_diff>
--- a/DataDrivenFrameWork/src/test/resources/excel/Testdata.xlsx
+++ b/DataDrivenFrameWork/src/test/resources/excel/Testdata.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baztronics\eclipse-workspace2\New folder\DataDrivenFrameWork\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baztronics\git\DataDrivenFrameWork\DataDrivenFrameWork\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>firstname</t>
   </si>
@@ -48,6 +49,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>asmaa dawood</t>
+  </si>
+  <si>
+    <t>Dollar</t>
   </si>
 </sst>
 </file>
@@ -368,7 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -405,4 +418,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Setting up run modes for Test Suites( Skipping Open Account Test)
</commit_message>
<xml_diff>
--- a/DataDrivenFrameWork/src/test/resources/excel/Testdata.xlsx
+++ b/DataDrivenFrameWork/src/test/resources/excel/Testdata.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>firstname</t>
   </si>
@@ -103,6 +104,27 @@
   </si>
   <si>
     <t>B5469</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -421,9 +443,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -532,7 +601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Setting up run modes for Test data (Skipped Test Case for Add Customer Test)
</commit_message>
<xml_diff>
--- a/DataDrivenFrameWork/src/test/resources/excel/Testdata.xlsx
+++ b/DataDrivenFrameWork/src/test/resources/excel/Testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>firstname</t>
   </si>
@@ -445,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -490,15 +490,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,8 +511,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -525,8 +528,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -539,8 +545,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -553,8 +562,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -567,8 +579,11 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -581,8 +596,11 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -594,6 +612,9 @@
       </c>
       <c r="D7" t="s">
         <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>